<commit_message>
Hoàn tất xuất bảng lương
</commit_message>
<xml_diff>
--- a/public/BANGLUONGTEMPLATE.xlsx
+++ b/public/BANGLUONGTEMPLATE.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/eproject-laravel/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1EEAFC-3AD3-D940-BB34-E4F77E4CB613}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B4CD14-6611-814E-992A-85CE7976979E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40960" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{9879CF8A-D84B-FF46-968C-5B781014FE06}"/>
+    <workbookView xWindow="1280" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{9879CF8A-D84B-FF46-968C-5B781014FE06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>STT</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Thuế TNCN</t>
   </si>
   <si>
-    <t>Khác (Bồi thường, BHYT, Thu hồi…)</t>
-  </si>
-  <si>
     <t>Lễ tết (300%)</t>
   </si>
   <si>
@@ -100,6 +97,75 @@
   </si>
   <si>
     <t>Phụ cấp</t>
+  </si>
+  <si>
+    <t>HO_VA_TEN</t>
+  </si>
+  <si>
+    <t>MA_SO</t>
+  </si>
+  <si>
+    <t>NGAY_VAO</t>
+  </si>
+  <si>
+    <t>CHUC_DANH</t>
+  </si>
+  <si>
+    <t>LUONG</t>
+  </si>
+  <si>
+    <t>NGAY_CONG</t>
+  </si>
+  <si>
+    <t>NGHI_CO_LUONG</t>
+  </si>
+  <si>
+    <t>THANH_TIEN</t>
+  </si>
+  <si>
+    <t>TG_100</t>
+  </si>
+  <si>
+    <t>TG_130</t>
+  </si>
+  <si>
+    <t>TG_200</t>
+  </si>
+  <si>
+    <t>TG_300</t>
+  </si>
+  <si>
+    <t>TONG_CONG_1</t>
+  </si>
+  <si>
+    <t>COM</t>
+  </si>
+  <si>
+    <t>DIEN_THOAI</t>
+  </si>
+  <si>
+    <t>XANG</t>
+  </si>
+  <si>
+    <t>TONG_CONG_2</t>
+  </si>
+  <si>
+    <t>BH</t>
+  </si>
+  <si>
+    <t>TNCN</t>
+  </si>
+  <si>
+    <t>TONG_CONG_3</t>
+  </si>
+  <si>
+    <t>THUC_LANH</t>
+  </si>
+  <si>
+    <t>Phòng ban</t>
+  </si>
+  <si>
+    <t>PHONG_BAN</t>
   </si>
 </sst>
 </file>
@@ -172,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -207,22 +273,54 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -235,7 +333,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -247,93 +345,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -342,75 +360,63 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -729,207 +735,282 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995A462D-D94C-2E43-ACD3-F65920864C42}">
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="18" t="s">
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="21" t="s">
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="23"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
       <c r="X1" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="56">
-      <c r="A2" s="9"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="1" t="s">
+    <row r="2" spans="1:24" ht="28">
+      <c r="A2" s="8"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="X2" s="6"/>
+    </row>
+    <row r="3" spans="1:24" ht="29">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>11</v>
+      </c>
+      <c r="L4">
+        <v>12</v>
+      </c>
+      <c r="M4">
+        <v>13</v>
+      </c>
+      <c r="N4">
+        <v>14</v>
+      </c>
+      <c r="O4">
+        <v>15</v>
+      </c>
+      <c r="P4">
+        <v>16</v>
+      </c>
+      <c r="Q4">
+        <v>17</v>
+      </c>
+      <c r="R4">
+        <v>18</v>
+      </c>
+      <c r="S4">
+        <v>19</v>
+      </c>
+      <c r="T4">
+        <v>20</v>
+      </c>
+      <c r="U4">
+        <v>21</v>
+      </c>
+      <c r="V4">
+        <v>22</v>
+      </c>
+      <c r="W4">
         <v>23</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="X2" s="7"/>
-    </row>
-    <row r="3" spans="1:24">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4">
-        <v>3</v>
-      </c>
-      <c r="D3" s="5">
-        <v>4</v>
-      </c>
-      <c r="E3" s="4">
-        <v>5</v>
-      </c>
-      <c r="F3" s="5">
-        <v>6</v>
-      </c>
-      <c r="G3" s="4">
-        <v>7</v>
-      </c>
-      <c r="H3" s="5">
-        <v>8</v>
-      </c>
-      <c r="I3" s="4">
-        <v>9</v>
-      </c>
-      <c r="J3" s="5">
-        <v>10</v>
-      </c>
-      <c r="K3" s="4">
-        <v>11</v>
-      </c>
-      <c r="L3" s="5">
-        <v>12</v>
-      </c>
-      <c r="M3" s="4">
-        <v>13</v>
-      </c>
-      <c r="N3" s="5">
-        <v>14</v>
-      </c>
-      <c r="O3" s="4">
-        <v>15</v>
-      </c>
-      <c r="P3" s="5">
-        <v>16</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>17</v>
-      </c>
-      <c r="R3" s="5">
-        <v>18</v>
-      </c>
-      <c r="S3" s="4">
-        <v>19</v>
-      </c>
-      <c r="T3" s="5">
-        <v>20</v>
-      </c>
-      <c r="U3" s="4">
-        <v>21</v>
-      </c>
-      <c r="V3" s="5">
-        <v>22</v>
-      </c>
-      <c r="W3" s="4">
-        <v>23</v>
-      </c>
-      <c r="X3" s="5">
+      <c r="X4">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="X1:X2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="U1:W1"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="T1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>